<commit_message>
structure codes withs full interfaces
</commit_message>
<xml_diff>
--- a/KylinGame/release/configfile/dataConfig/tollgate/tollgateSheetData.xlsx
+++ b/KylinGame/release/configfile/dataConfig/tollgate/tollgateSheetData.xlsx
@@ -1,10 +1,10 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="4" rupBuild="9302"/>
+  <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4505"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="90" windowWidth="19200" windowHeight="11640" activeTab="4"/>
+    <workbookView xWindow="0" yWindow="90" windowWidth="19200" windowHeight="11640"/>
   </bookViews>
   <sheets>
     <sheet name="tollgateSheetData" sheetId="1" r:id="rId1"/>
@@ -16,7 +16,7 @@
   <definedNames>
     <definedName name="_xlnm._FilterDatabase" localSheetId="3" hidden="1">dropInfo!$A$1:$AW$153</definedName>
   </definedNames>
-  <calcPr calcId="145621"/>
+  <calcPr calcId="124519"/>
 </workbook>
 </file>
 
@@ -4234,18 +4234,10 @@
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
-    <t>该关卡不能建的塔</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
     <t>建塔最高等级</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
-    <t>towerLocked</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
     <t>maxTowerLvl</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
@@ -4255,13 +4247,21 @@
   </si>
   <si>
     <t>probability</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>1:10;2:10;3:10;4:10</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>1:0;2:3;3:1;4:0</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <numFmts count="1">
     <numFmt numFmtId="176" formatCode="0.00_ "/>
   </numFmts>
@@ -4720,7 +4720,7 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office 主题​​">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office 主题">
   <a:themeElements>
     <a:clrScheme name="Office">
       <a:dk1>
@@ -4794,7 +4794,6 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
-        <a:font script="Geor" typeface="Sylfaen"/>
       </a:majorFont>
       <a:minorFont>
         <a:latin typeface="Calibri"/>
@@ -4829,7 +4828,6 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
-        <a:font script="Geor" typeface="Sylfaen"/>
       </a:minorFont>
     </a:fontScheme>
     <a:fmtScheme name="Office">
@@ -5005,12 +5003,12 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:AJ138"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <dimension ref="A1:AI138"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView tabSelected="1" workbookViewId="0">
       <pane xSplit="1" topLeftCell="V1" activePane="topRight" state="frozen"/>
-      <selection pane="topRight" activeCell="AJ5" sqref="AJ5"/>
+      <selection pane="topRight" activeCell="AI16" sqref="AI16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.5"/>
@@ -5046,12 +5044,11 @@
     <col min="30" max="30" width="16.125" style="1" bestFit="1" customWidth="1"/>
     <col min="31" max="31" width="16.125" style="1" customWidth="1"/>
     <col min="32" max="34" width="17.5" style="1" customWidth="1"/>
-    <col min="35" max="35" width="20.875" style="50" customWidth="1"/>
-    <col min="36" max="36" width="14.625" style="50" customWidth="1"/>
-    <col min="37" max="16384" width="9" style="50"/>
+    <col min="35" max="35" width="19.625" style="50" customWidth="1"/>
+    <col min="36" max="16384" width="9" style="50"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:36">
+    <row r="1" spans="1:35">
       <c r="A1" s="2" t="s">
         <v>0</v>
       </c>
@@ -5157,11 +5154,8 @@
       <c r="AI1" s="50" t="s">
         <v>637</v>
       </c>
-      <c r="AJ1" s="50" t="s">
-        <v>638</v>
-      </c>
-    </row>
-    <row r="2" spans="1:36">
+    </row>
+    <row r="2" spans="1:35">
       <c r="A2" s="4" t="s">
         <v>24</v>
       </c>
@@ -5265,13 +5259,10 @@
         <v>413</v>
       </c>
       <c r="AI2" s="50" t="s">
-        <v>639</v>
-      </c>
-      <c r="AJ2" s="50" t="s">
-        <v>640</v>
-      </c>
-    </row>
-    <row r="3" spans="1:36" s="1" customFormat="1">
+        <v>638</v>
+      </c>
+    </row>
+    <row r="3" spans="1:35" s="1" customFormat="1">
       <c r="A3" s="6" t="s">
         <v>382</v>
       </c>
@@ -5362,8 +5353,11 @@
       <c r="AH3" s="7">
         <v>1</v>
       </c>
-    </row>
-    <row r="4" spans="1:36">
+      <c r="AI3" s="1" t="s">
+        <v>641</v>
+      </c>
+    </row>
+    <row r="4" spans="1:35">
       <c r="A4" s="6">
         <v>100110111</v>
       </c>
@@ -5464,8 +5458,11 @@
       <c r="AH4" s="7">
         <v>1</v>
       </c>
-    </row>
-    <row r="5" spans="1:36">
+      <c r="AI4" s="50" t="s">
+        <v>642</v>
+      </c>
+    </row>
+    <row r="5" spans="1:35">
       <c r="A5" s="6">
         <v>100110112</v>
       </c>
@@ -5569,7 +5566,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="6" spans="1:36">
+    <row r="6" spans="1:35">
       <c r="A6" s="6">
         <v>100110113</v>
       </c>
@@ -5673,7 +5670,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="7" spans="1:36">
+    <row r="7" spans="1:35">
       <c r="A7" s="6">
         <v>100110211</v>
       </c>
@@ -5778,7 +5775,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="8" spans="1:36">
+    <row r="8" spans="1:35">
       <c r="A8" s="6">
         <v>100110212</v>
       </c>
@@ -5885,7 +5882,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="9" spans="1:36">
+    <row r="9" spans="1:35">
       <c r="A9" s="6">
         <v>100110213</v>
       </c>
@@ -5992,7 +5989,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="10" spans="1:36">
+    <row r="10" spans="1:35">
       <c r="A10" s="6">
         <v>100110311</v>
       </c>
@@ -6097,7 +6094,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="11" spans="1:36">
+    <row r="11" spans="1:35">
       <c r="A11" s="6">
         <v>100110312</v>
       </c>
@@ -6204,7 +6201,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="12" spans="1:36">
+    <row r="12" spans="1:35">
       <c r="A12" s="6">
         <v>100110313</v>
       </c>
@@ -6311,7 +6308,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="13" spans="1:36">
+    <row r="13" spans="1:35">
       <c r="A13" s="6" t="s">
         <v>52</v>
       </c>
@@ -6416,7 +6413,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="14" spans="1:36">
+    <row r="14" spans="1:35">
       <c r="A14" s="6">
         <v>100110412</v>
       </c>
@@ -6523,7 +6520,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="15" spans="1:36">
+    <row r="15" spans="1:35">
       <c r="A15" s="6">
         <v>100110413</v>
       </c>
@@ -6630,7 +6627,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="16" spans="1:36">
+    <row r="16" spans="1:35">
       <c r="A16" s="6" t="s">
         <v>55</v>
       </c>
@@ -19789,7 +19786,7 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:B12"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -19903,7 +19900,7 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:F63"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -21177,7 +21174,7 @@
 </file>
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:AW153"/>
   <sheetViews>
     <sheetView topLeftCell="A104" workbookViewId="0">
@@ -27487,10 +27484,10 @@
 </file>
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:C153"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="C4" sqref="C4"/>
     </sheetView>
   </sheetViews>
@@ -27517,10 +27514,10 @@
         <v>24</v>
       </c>
       <c r="B2" s="40" t="s">
-        <v>641</v>
+        <v>639</v>
       </c>
       <c r="C2" s="40" t="s">
-        <v>642</v>
+        <v>640</v>
       </c>
     </row>
     <row r="3" spans="1:3">

</xml_diff>